<commit_message>
mher: Updated ToDo list.
</commit_message>
<xml_diff>
--- a/final/todo.xlsx
+++ b/final/todo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>TODO:</t>
   </si>
@@ -132,13 +132,16 @@
   </si>
   <si>
     <t>Guru</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +172,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +190,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,11 +216,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -213,8 +229,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Gut" xfId="2" builtinId="26"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -497,7 +515,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,8 +687,8 @@
       <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>31</v>
+      <c r="G11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -709,8 +727,8 @@
       <c r="F13" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>31</v>
+      <c r="G13" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mher: Updates and fixes all around.
</commit_message>
<xml_diff>
--- a/final/todo.xlsx
+++ b/final/todo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>TODO:</t>
   </si>
@@ -135,13 +135,16 @@
   </si>
   <si>
     <t>Implement backspace, more functionality</t>
+  </si>
+  <si>
+    <t>Skipped</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,8 +182,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +205,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -216,12 +231,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -230,9 +246,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Gut" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -515,7 +533,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,8 +605,8 @@
       <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>30</v>
+      <c r="G6" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -667,8 +685,8 @@
       <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>30</v>
+      <c r="G10" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mher: Test for getdents.
</commit_message>
<xml_diff>
--- a/final/todo.xlsx
+++ b/final/todo.xlsx
@@ -74,9 +74,6 @@
     <t>Improve file hiding</t>
   </si>
   <si>
-    <t>Improve overall, get rid of used syscall in kernel space</t>
-  </si>
-  <si>
     <t>Improve hiding sockets</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Skipped</t>
+  </si>
+  <si>
+    <t>Improve overall[, get rid of used syscall in kernel space]</t>
   </si>
 </sst>
 </file>
@@ -530,11 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -578,19 +577,19 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="3">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -604,10 +603,10 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -624,13 +623,13 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>4</v>
       </c>
@@ -644,10 +643,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -658,56 +657,56 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>7</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -715,39 +714,39 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
       </c>
       <c r="E12" s="3">
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>9</v>
       </c>
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
         <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -755,19 +754,19 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -775,19 +774,19 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -795,29 +794,23 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:G16">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="No"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B4:G16"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>